<commit_message>
worked on TestDetector and Report generation
</commit_message>
<xml_diff>
--- a/excel/testData.xlsx
+++ b/excel/testData.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25915"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45E08902-9E1D-499A-A905-C51923043149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A07E425-D384-45C7-BA9A-C44E506D970F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
     <sheet name="flags" sheetId="2" r:id="rId2"/>
-    <sheet name="sites" sheetId="3" r:id="rId3"/>
+    <sheet name="logins" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -92,35 +93,23 @@
     <t>japan</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Element</t>
-  </si>
-  <si>
-    <t>https://github.com/dhatim/fastexcel</t>
-  </si>
-  <si>
-    <t>Parabank</t>
-  </si>
-  <si>
-    <t>https://parabank.parasoft.com/parabank/index.htm</t>
-  </si>
-  <si>
-    <t>CiCd</t>
-  </si>
-  <si>
-    <t>https://parabank.parasoft.com/just/making/itlong/parabank/index.htm</t>
+    <t>kaiser.bobo</t>
+  </si>
+  <si>
+    <t>cutie.pie.bb2022</t>
+  </si>
+  <si>
+    <t>guligina.beauty</t>
+  </si>
+  <si>
+    <t>only1wife2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,14 +121,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,17 +143,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -601,56 +579,55 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F08ADE-7D7E-4033-A8A8-C95DE2763AB8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="66.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{E604DE20-6F24-4CF1-AEA1-548C94C41455}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{4D0572E6-4E91-4831-A5FF-3EE3C2B67DFD}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{BF9D10A8-695C-4C52-AECF-B4F18D722168}"/>
-  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB656C59-4FBF-4EE0-AD5F-A0B710608163}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>